<commit_message>
removed totals from financial graphs
</commit_message>
<xml_diff>
--- a/server/src/static/pwidexample.xlsx
+++ b/server/src/static/pwidexample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="21620" windowHeight="13680" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="21620" windowHeight="13680" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
     <sheet name="Economics and costs" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -33,6 +33,270 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="146">
   <si>
+    <t>If you have any questions, please contact us on</t>
+  </si>
+  <si>
+    <t>info@optimamodel.com</t>
+  </si>
+  <si>
+    <t>Populations</t>
+  </si>
+  <si>
+    <t>Short name</t>
+  </si>
+  <si>
+    <t>Long name</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Has sex with men</t>
+  </si>
+  <si>
+    <t>Has sex with women</t>
+  </si>
+  <si>
+    <t>Sex worker</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>PWID</t>
+  </si>
+  <si>
+    <t>People who inject drugs</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Average number of injections per person per year</t>
+  </si>
+  <si>
+    <t>Average percentage of people who receptively shared a needle/syringe at last injection</t>
+  </si>
+  <si>
+    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
+  </si>
+  <si>
+    <t>Interactions between regular partners</t>
+  </si>
+  <si>
+    <t>Interactions between casual partners</t>
+  </si>
+  <si>
+    <t>O P T I M A</t>
+  </si>
+  <si>
+    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet looks complicated and confusing. Unfortunately, it is. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
+  </si>
+  <si>
+    <t>I. LAYOUT OF THE SPREADSHEET</t>
+  </si>
+  <si>
+    <t>This spreadsheet is divided into 12 sheets. All sheets need to be completed, except where noted below.</t>
+  </si>
+  <si>
+    <t>II. HOW TO ENTER DATA</t>
+  </si>
+  <si>
+    <t>Do not enter anything except actual data, apart from the small number of instances which allows optional input of output from other models for comparison and verification! Optima will fit to actual data and will interpolate between data points, so only enter data in the years that they belong. In addition, please feel free to add notes (either as comments for a given cell or in the blank cells to the right of each row) about the source of the data.</t>
+  </si>
+  <si>
+    <t>III. WHAT CAN BE LEFT BLANK</t>
+  </si>
+  <si>
+    <t>It can be confusing what can and cannot be left blank, but here are a few general principles:</t>
+  </si>
+  <si>
+    <t>* Nothing on the "Populations and programs" sheet can be blank.</t>
+  </si>
+  <si>
+    <t>* For each parameter (as in, row in the worksheet), there needs to be at least one data point entered. The only exception to this is the sheet "Optional indicators", which may be left blank. If data are not available for a particular indicator, enter an assumption in the "Assumption" column, with a comment explaining how that value was derived.</t>
+  </si>
+  <si>
+    <t>* Economic data only need to be entered if you are performing economic analyses.</t>
+  </si>
+  <si>
+    <t>If a parameter is left completely blank, it will be assumed to be zero.</t>
+  </si>
+  <si>
+    <t>IV. QUESTIONS</t>
+  </si>
+  <si>
+    <t>Untreated HIV, CD4(50-200)</t>
+  </si>
+  <si>
+    <t>Untreated HIV, CD4(&lt;50)</t>
+  </si>
+  <si>
+    <t>Treated HIV</t>
+  </si>
+  <si>
+    <t>Consumer price index</t>
+  </si>
+  <si>
+    <t>Growth assumptions</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Purchasing power parity</t>
+  </si>
+  <si>
+    <t>Gross domestic product</t>
+  </si>
+  <si>
+    <t>Government revenue</t>
+  </si>
+  <si>
+    <t>Government expenditure</t>
+  </si>
+  <si>
+    <t>Total domestic and international health expenditure</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>NSP</t>
+  </si>
+  <si>
+    <t>Needle-syringe program</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>Antiretroviral therapy</t>
+  </si>
+  <si>
+    <t>Cost &amp; coverage</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Population size</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>HIV prevalence</t>
+  </si>
+  <si>
+    <t>Number of HIV tests per year</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Number of HIV diagnoses per year</t>
+  </si>
+  <si>
+    <t>Modeled estimate of new HIV infections per year</t>
+  </si>
+  <si>
+    <t>Modeled estimate of HIV prevalence</t>
+  </si>
+  <si>
+    <t>Number of HIV-related deaths</t>
+  </si>
+  <si>
+    <t>Number of people initiating ART each year</t>
+  </si>
+  <si>
+    <t>Percentage of people who die from non-HIV-related causes per year</t>
+  </si>
+  <si>
+    <t>Prevalence of any ulcerative STIs</t>
+  </si>
+  <si>
+    <t>Prevalence of any discharging STIs</t>
+  </si>
+  <si>
+    <t>Tuberculosis prevalence</t>
+  </si>
+  <si>
+    <t>Percentage of population tested for HIV in the last 12 months</t>
+  </si>
+  <si>
+    <t>Probability of a person with CD4 &lt;200 being tested per year</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Number of people on first-line treatment</t>
+  </si>
+  <si>
+    <t>Number of people on subsequent lines of treatment</t>
+  </si>
+  <si>
+    <t>Treatment eligibility criterion</t>
+  </si>
+  <si>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Number (or percentage) of women on PMTCT (Option B/B+)</t>
+  </si>
+  <si>
+    <t>Birth rate (births per woman per year)</t>
+  </si>
+  <si>
+    <t>Percentage of HIV-positive women who breastfeed</t>
+  </si>
+  <si>
+    <t>Average number of acts with regular partners per person per year</t>
+  </si>
+  <si>
+    <t>Average number of acts with casual partners per person per year</t>
+  </si>
+  <si>
+    <t>Average number of acts with commercial partners per person per year</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with casual partners</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with commercial partners</t>
+  </si>
+  <si>
+    <t>Percentage of males who have been circumcised</t>
+  </si>
+  <si>
     <t>General government health expenditure</t>
   </si>
   <si>
@@ -205,281 +469,16 @@
   </si>
   <si>
     <t>Untreated HIV, CD4(200-350)</t>
-  </si>
-  <si>
-    <t>Untreated HIV, CD4(50-200)</t>
-  </si>
-  <si>
-    <t>Untreated HIV, CD4(&lt;50)</t>
-  </si>
-  <si>
-    <t>Treated HIV</t>
-  </si>
-  <si>
-    <t>Consumer price index</t>
-  </si>
-  <si>
-    <t>Growth assumptions</t>
-  </si>
-  <si>
-    <t>AND</t>
-  </si>
-  <si>
-    <t>Purchasing power parity</t>
-  </si>
-  <si>
-    <t>Gross domestic product</t>
-  </si>
-  <si>
-    <t>Government revenue</t>
-  </si>
-  <si>
-    <t>Government expenditure</t>
-  </si>
-  <si>
-    <t>Total domestic and international health expenditure</t>
-  </si>
-  <si>
-    <t>Programs</t>
-  </si>
-  <si>
-    <t>NSP</t>
-  </si>
-  <si>
-    <t>Needle-syringe program</t>
-  </si>
-  <si>
-    <t>ART</t>
-  </si>
-  <si>
-    <t>Antiretroviral therapy</t>
-  </si>
-  <si>
-    <t>Cost &amp; coverage</t>
-  </si>
-  <si>
-    <t>Assumption</t>
-  </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Population size</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>best</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>HIV prevalence</t>
-  </si>
-  <si>
-    <t>Number of HIV tests per year</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Number of HIV diagnoses per year</t>
-  </si>
-  <si>
-    <t>Modeled estimate of new HIV infections per year</t>
-  </si>
-  <si>
-    <t>Modeled estimate of HIV prevalence</t>
-  </si>
-  <si>
-    <t>Number of HIV-related deaths</t>
-  </si>
-  <si>
-    <t>Number of people initiating ART each year</t>
-  </si>
-  <si>
-    <t>Percentage of people who die from non-HIV-related causes per year</t>
-  </si>
-  <si>
-    <t>Prevalence of any ulcerative STIs</t>
-  </si>
-  <si>
-    <t>Prevalence of any discharging STIs</t>
-  </si>
-  <si>
-    <t>Tuberculosis prevalence</t>
-  </si>
-  <si>
-    <t>Percentage of population tested for HIV in the last 12 months</t>
-  </si>
-  <si>
-    <t>Probability of a person with CD4 &lt;200 being tested per year</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Number of people on first-line treatment</t>
-  </si>
-  <si>
-    <t>Number of people on subsequent lines of treatment</t>
-  </si>
-  <si>
-    <t>Treatment eligibility criterion</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Number (or percentage) of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
-    <t>Birth rate (births per woman per year)</t>
-  </si>
-  <si>
-    <t>Percentage of HIV-positive women who breastfeed</t>
-  </si>
-  <si>
-    <t>Average number of acts with regular partners per person per year</t>
-  </si>
-  <si>
-    <t>Average number of acts with casual partners per person per year</t>
-  </si>
-  <si>
-    <t>Average number of acts with commercial partners per person per year</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with casual partners</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with commercial partners</t>
-  </si>
-  <si>
-    <t>Percentage of males who have been circumcised</t>
-  </si>
-  <si>
-    <t>Average number of injections per person per year</t>
-  </si>
-  <si>
-    <t>Average percentage of people who receptively shared a needle/syringe at last injection</t>
-  </si>
-  <si>
-    <t>Number of people who inject drugs who are on opiate substitution therapy</t>
-  </si>
-  <si>
-    <t>Interactions between regular partners</t>
-  </si>
-  <si>
-    <t>Interactions between casual partners</t>
-  </si>
-  <si>
-    <t>O P T I M A</t>
-  </si>
-  <si>
-    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet looks complicated and confusing. Unfortunately, it is. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
-  </si>
-  <si>
-    <t>I. LAYOUT OF THE SPREADSHEET</t>
-  </si>
-  <si>
-    <t>This spreadsheet is divided into 12 sheets. All sheets need to be completed, except where noted below.</t>
-  </si>
-  <si>
-    <t>II. HOW TO ENTER DATA</t>
-  </si>
-  <si>
-    <t>Do not enter anything except actual data, apart from the small number of instances which allows optional input of output from other models for comparison and verification! Optima will fit to actual data and will interpolate between data points, so only enter data in the years that they belong. In addition, please feel free to add notes (either as comments for a given cell or in the blank cells to the right of each row) about the source of the data.</t>
-  </si>
-  <si>
-    <t>III. WHAT CAN BE LEFT BLANK</t>
-  </si>
-  <si>
-    <t>It can be confusing what can and cannot be left blank, but here are a few general principles:</t>
-  </si>
-  <si>
-    <t>* Nothing on the "Populations and programs" sheet can be blank.</t>
-  </si>
-  <si>
-    <t>* For each parameter (as in, row in the worksheet), there needs to be at least one data point entered. The only exception to this is the sheet "Optional indicators", which may be left blank. If data are not available for a particular indicator, enter an assumption in the "Assumption" column, with a comment explaining how that value was derived.</t>
-  </si>
-  <si>
-    <t>* Economic data only need to be entered if you are performing economic analyses.</t>
-  </si>
-  <si>
-    <t>If a parameter is left completely blank, it will be assumed to be zero.</t>
-  </si>
-  <si>
-    <t>IV. QUESTIONS</t>
-  </si>
-  <si>
-    <t>If you have any questions, please contact us on</t>
-  </si>
-  <si>
-    <t>info@optimamodel.com</t>
-  </si>
-  <si>
-    <t>Populations</t>
-  </si>
-  <si>
-    <t>Short name</t>
-  </si>
-  <si>
-    <t>Long name</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Has sex with men</t>
-  </si>
-  <si>
-    <t>Has sex with women</t>
-  </si>
-  <si>
-    <t>Sex worker</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>PWID</t>
-  </si>
-  <si>
-    <t>People who inject drugs</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -646,9 +645,6 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -671,8 +667,11 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,22 +981,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
-        <v>117</v>
+      <c r="A1" s="22" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="13"/>
+      <c r="A2" s="22"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="22"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:1" ht="65" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -1005,7 +1004,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1013,7 +1012,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1021,7 +1020,7 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -1029,7 +1028,7 @@
     </row>
     <row r="13" spans="1:1" ht="80" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -1037,7 +1036,7 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -1045,22 +1044,22 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>124</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="57" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -1068,7 +1067,7 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1">
@@ -1076,7 +1075,7 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:1">
@@ -1084,7 +1083,7 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -1092,7 +1091,7 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -1131,7 +1130,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1151,7 +1150,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1171,7 +1170,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1189,7 +1188,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1234,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1252,7 +1251,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1293,23 +1292,23 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="C2" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="C3" s="8">
         <v>4.0000000000000002E-4</v>
@@ -1323,7 +1322,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C4" s="8">
         <v>8.0000000000000004E-4</v>
@@ -1337,7 +1336,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="C5" s="8">
         <v>1.38E-2</v>
@@ -1351,7 +1350,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="C6" s="8">
         <v>1.1000000000000001E-3</v>
@@ -1365,7 +1364,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="C7" s="8">
         <v>8.0000000000000002E-3</v>
@@ -1379,7 +1378,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C8" s="8">
         <v>0.36699999999999999</v>
@@ -1393,7 +1392,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="C9" s="8">
         <v>0.20499999999999999</v>
@@ -1407,23 +1406,23 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C15" s="11">
         <v>26.03</v>
@@ -1437,7 +1436,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
@@ -1451,7 +1450,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C17" s="11">
         <v>1</v>
@@ -1465,7 +1464,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
@@ -1479,7 +1478,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C19" s="11">
         <v>3.49</v>
@@ -1493,7 +1492,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C20" s="11">
         <v>7.17</v>
@@ -1507,23 +1506,23 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="C25" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>116</v>
       </c>
       <c r="C26" s="12">
         <v>4.1399999999999997</v>
@@ -1537,7 +1536,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="5" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C27" s="12">
         <v>1.05</v>
@@ -1551,7 +1550,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="5" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="C28" s="12">
         <v>0.33</v>
@@ -1565,7 +1564,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="5" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="C29" s="12">
         <v>0.27</v>
@@ -1579,7 +1578,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="C30" s="12">
         <v>0.67</v>
@@ -1593,23 +1592,23 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="C35" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="5" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C36" s="12">
         <v>0.45</v>
@@ -1623,7 +1622,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="5" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C37" s="12">
         <v>0.7</v>
@@ -1637,7 +1636,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="5" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="C38" s="12">
         <v>0.47</v>
@@ -1651,7 +1650,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="B39" s="5" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="C39" s="12">
         <v>1.52</v>
@@ -1665,23 +1664,23 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="C44" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="B45" s="5" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="C45" s="12">
         <v>0.1</v>
@@ -1695,7 +1694,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="B46" s="5" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="C46" s="12">
         <v>0.16</v>
@@ -1709,23 +1708,23 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="C51" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="B52" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C52" s="8">
         <v>3.5999999999999999E-3</v>
@@ -1739,7 +1738,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="B53" s="5" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="C53" s="8">
         <v>3.5999999999999999E-3</v>
@@ -1753,7 +1752,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="B54" s="5" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="C54" s="8">
         <v>5.7999999999999996E-3</v>
@@ -1767,7 +1766,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="B55" s="5" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C55" s="8">
         <v>8.8000000000000005E-3</v>
@@ -1781,7 +1780,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="B56" s="5" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C56" s="8">
         <v>5.8999999999999997E-2</v>
@@ -1795,7 +1794,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="B57" s="5" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C57" s="8">
         <v>0.32300000000000001</v>
@@ -1809,7 +1808,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="B58" s="5" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C58" s="8">
         <v>0.23</v>
@@ -1823,7 +1822,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="B59" s="5" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="C59" s="8">
         <v>2.17</v>
@@ -1837,23 +1836,23 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="C64" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="B65" s="5" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="C65" s="12">
         <v>0.05</v>
@@ -1867,7 +1866,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="B66" s="5" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="C66" s="12">
         <v>0.42</v>
@@ -1881,7 +1880,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="B67" s="5" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="C67" s="12">
         <v>1</v>
@@ -1895,7 +1894,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="B68" s="5" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="C68" s="12">
         <v>2.65</v>
@@ -1909,7 +1908,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="B69" s="5" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="C69" s="12">
         <v>1</v>
@@ -1923,7 +1922,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="B70" s="5" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="C70" s="12">
         <v>0.46</v>
@@ -1937,7 +1936,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="B71" s="5" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="C71" s="12">
         <v>0.1</v>
@@ -1951,7 +1950,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="B72" s="5" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C72" s="12">
         <v>0.3</v>
@@ -1965,7 +1964,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="B73" s="5" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="C73" s="12">
         <v>0.27500000000000002</v>
@@ -1979,23 +1978,23 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="4" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="C78" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="B79" s="5" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="C79" s="11">
         <v>0.14599999999999999</v>
@@ -2009,7 +2008,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="B80" s="5" t="s">
-        <v>55</v>
+        <v>143</v>
       </c>
       <c r="C80" s="11">
         <v>8.0000000000000002E-3</v>
@@ -2023,7 +2022,7 @@
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="5" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="C81" s="11">
         <v>0.02</v>
@@ -2037,7 +2036,7 @@
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="5" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="C82" s="11">
         <v>7.0000000000000007E-2</v>
@@ -2051,7 +2050,7 @@
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C83" s="11">
         <v>0.26500000000000001</v>
@@ -2065,7 +2064,7 @@
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="5" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C84" s="11">
         <v>0.54700000000000004</v>
@@ -2079,7 +2078,7 @@
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="5" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C85" s="11">
         <v>5.2999999999999999E-2</v>
@@ -2115,10 +2114,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -2171,71 +2170,71 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="B3" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="16">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15">
         <v>75.018454192929113</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>76.070810544531554</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>77.902335510111072</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>79.45534236885652</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>81.068347459232555</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>82.769770996223016</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <v>84.249516856345011</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <v>85.442534325304138</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="15">
         <v>89.999873687933118</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <v>89.504730386893897</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <v>92.521062537104171</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="15">
         <v>95.719284063206572</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <v>98.951609847288623</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <v>100</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <f>P3*(1.025)</f>
         <v>102.49999999999999</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="15">
         <f>Q3*(1.025)</f>
         <v>105.06249999999997</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T3" s="12">
         <v>0.03</v>
@@ -2249,7 +2248,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -2302,18 +2301,18 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="B9" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2332,7 +2331,7 @@
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
       <c r="S9" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
@@ -2340,7 +2339,7 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="4" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -2393,85 +2392,85 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="B15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="16">
+        <v>61</v>
+      </c>
+      <c r="C15" s="15">
         <f t="shared" ref="C15:Q15" si="0">D15/(1.12)</f>
         <v>529043227.23311073</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <f t="shared" si="0"/>
         <v>592528414.50108409</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <f t="shared" si="0"/>
         <v>663631824.24121428</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <f t="shared" si="0"/>
         <v>743267643.15016007</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <f t="shared" si="0"/>
         <v>832459760.32817936</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <f t="shared" si="0"/>
         <v>932354931.56756091</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <f t="shared" si="0"/>
         <v>1044237523.3556683</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="15">
         <f t="shared" si="0"/>
         <v>1169546026.1583486</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="15">
         <f t="shared" si="0"/>
         <v>1309891549.2973506</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="15">
         <f t="shared" si="0"/>
         <v>1467078535.213033</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <f t="shared" si="0"/>
         <v>1643127959.438597</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N15" s="15">
         <f t="shared" si="0"/>
         <v>1840303314.5712287</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="15">
         <f t="shared" si="0"/>
         <v>2061139712.3197763</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="15">
         <f t="shared" si="0"/>
         <v>2308476477.7981496</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15" s="15">
         <f t="shared" si="0"/>
         <v>2585493655.1339278</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="15">
         <f>3243243241/(1.12)</f>
         <v>2895752893.7499995</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T15" s="12">
         <v>0.04</v>
@@ -2485,7 +2484,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -2538,84 +2537,84 @@
         <v>2015</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V20" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:22">
       <c r="B21" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="17">
+        <v>61</v>
+      </c>
+      <c r="C21" s="16">
         <v>30000000000</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <f>C21+5000000000</f>
         <v>35000000000</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <f t="shared" ref="E21:R21" si="1">D21+5000000000</f>
         <v>40000000000</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="16">
         <f t="shared" si="1"/>
         <v>45000000000</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="16">
         <f t="shared" si="1"/>
         <v>50000000000</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="16">
         <f t="shared" si="1"/>
         <v>55000000000</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="16">
         <f t="shared" si="1"/>
         <v>60000000000</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="16">
         <f t="shared" si="1"/>
         <v>65000000000</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="16">
         <f t="shared" si="1"/>
         <v>70000000000</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="16">
         <f t="shared" si="1"/>
         <v>75000000000</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="16">
         <f t="shared" si="1"/>
         <v>80000000000</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="16">
         <f t="shared" si="1"/>
         <v>85000000000</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="16">
         <f t="shared" si="1"/>
         <v>90000000000</v>
       </c>
-      <c r="P21" s="17">
+      <c r="P21" s="16">
         <f t="shared" si="1"/>
         <v>95000000000</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="16">
         <f t="shared" si="1"/>
         <v>100000000000</v>
       </c>
-      <c r="R21" s="17">
+      <c r="R21" s="16">
         <f t="shared" si="1"/>
         <v>105000000000</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T21" s="8">
         <v>3.5000000000000003E-2</v>
@@ -2629,7 +2628,7 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="4" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -2682,69 +2681,69 @@
         <v>2015</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V26" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="B27" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="18">
+        <v>61</v>
+      </c>
+      <c r="C27" s="17">
         <v>30000000000</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="17">
         <v>35000000000</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="17">
         <v>40000000000</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="17">
         <v>45000000000</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="17">
         <v>50000000000</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="17">
         <v>55000000000</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="17">
         <v>60000000000</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="17">
         <v>65000000000</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="17">
         <v>70000000000</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="17">
         <v>75000000000</v>
       </c>
-      <c r="M27" s="18">
+      <c r="M27" s="17">
         <v>80000000000</v>
       </c>
-      <c r="N27" s="18">
+      <c r="N27" s="17">
         <v>85000000000</v>
       </c>
-      <c r="O27" s="18">
+      <c r="O27" s="17">
         <v>90000000000</v>
       </c>
-      <c r="P27" s="18">
+      <c r="P27" s="17">
         <v>95000000000</v>
       </c>
-      <c r="Q27" s="18">
+      <c r="Q27" s="17">
         <v>100000000000</v>
       </c>
-      <c r="R27" s="18">
+      <c r="R27" s="17">
         <v>105000000000</v>
       </c>
       <c r="S27" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T27" s="12">
         <v>0.03</v>
@@ -2758,7 +2757,7 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -2811,18 +2810,18 @@
         <v>2015</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U32" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="B33" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C33" s="10">
         <f>C39*1.25</f>
@@ -2889,7 +2888,7 @@
         <v>15750000000</v>
       </c>
       <c r="S33" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T33" s="8">
         <v>2.5000000000000001E-2</v>
@@ -2903,7 +2902,7 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="4" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -2956,85 +2955,85 @@
         <v>2015</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U38" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V38" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:22">
       <c r="B39" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="16">
+        <v>61</v>
+      </c>
+      <c r="C39" s="15">
         <f>12%*C27</f>
         <v>3600000000</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="15">
         <f t="shared" ref="D39:R39" si="3">12%*D27</f>
         <v>4200000000</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="15">
         <f t="shared" si="3"/>
         <v>4800000000</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="15">
         <f t="shared" si="3"/>
         <v>5400000000</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="15">
         <f t="shared" si="3"/>
         <v>6000000000</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="15">
         <f t="shared" si="3"/>
         <v>6600000000</v>
       </c>
-      <c r="I39" s="16">
+      <c r="I39" s="15">
         <f t="shared" si="3"/>
         <v>7200000000</v>
       </c>
-      <c r="J39" s="16">
+      <c r="J39" s="15">
         <f t="shared" si="3"/>
         <v>7800000000</v>
       </c>
-      <c r="K39" s="16">
+      <c r="K39" s="15">
         <f t="shared" si="3"/>
         <v>8400000000</v>
       </c>
-      <c r="L39" s="16">
+      <c r="L39" s="15">
         <f t="shared" si="3"/>
         <v>9000000000</v>
       </c>
-      <c r="M39" s="16">
+      <c r="M39" s="15">
         <f t="shared" si="3"/>
         <v>9600000000</v>
       </c>
-      <c r="N39" s="16">
+      <c r="N39" s="15">
         <f t="shared" si="3"/>
         <v>10200000000</v>
       </c>
-      <c r="O39" s="16">
+      <c r="O39" s="15">
         <f t="shared" si="3"/>
         <v>10800000000</v>
       </c>
-      <c r="P39" s="16">
+      <c r="P39" s="15">
         <f t="shared" si="3"/>
         <v>11400000000</v>
       </c>
-      <c r="Q39" s="16">
+      <c r="Q39" s="15">
         <f t="shared" si="3"/>
         <v>12000000000</v>
       </c>
-      <c r="R39" s="16">
+      <c r="R39" s="15">
         <f t="shared" si="3"/>
         <v>12600000000</v>
       </c>
       <c r="S39" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T39" s="8">
         <v>2.5000000000000001E-2</v>
@@ -3048,7 +3047,7 @@
     </row>
     <row r="43" spans="1:22">
       <c r="A43" s="4" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -3101,83 +3100,83 @@
         <v>2015</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U44" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V44" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:22">
       <c r="B45" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="16">
+        <v>61</v>
+      </c>
+      <c r="C45" s="15">
         <v>15000000</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="15">
         <v>16000000</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="15">
         <v>17000000</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="15">
         <v>18000000</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="15">
         <v>18000000</v>
       </c>
-      <c r="H45" s="16">
+      <c r="H45" s="15">
         <v>18000000</v>
       </c>
-      <c r="I45" s="16">
+      <c r="I45" s="15">
         <v>18000000</v>
       </c>
-      <c r="J45" s="16">
+      <c r="J45" s="15">
         <v>18000000</v>
       </c>
-      <c r="K45" s="16">
+      <c r="K45" s="15">
         <v>18000000</v>
       </c>
-      <c r="L45" s="16">
+      <c r="L45" s="15">
         <v>18000000</v>
       </c>
-      <c r="M45" s="16">
+      <c r="M45" s="15">
         <v>18000000</v>
       </c>
-      <c r="N45" s="16">
+      <c r="N45" s="15">
         <v>18000000</v>
       </c>
-      <c r="O45" s="16">
+      <c r="O45" s="15">
         <v>18000000</v>
       </c>
-      <c r="P45" s="16">
+      <c r="P45" s="15">
         <v>18000000</v>
       </c>
-      <c r="Q45" s="16">
+      <c r="Q45" s="15">
         <v>18000000</v>
       </c>
-      <c r="R45" s="16">
+      <c r="R45" s="15">
         <v>18000000</v>
       </c>
-      <c r="S45" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="T45" s="20">
+      <c r="S45" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T45" s="19">
         <v>0.03</v>
       </c>
-      <c r="U45" s="20">
+      <c r="U45" s="19">
         <v>0.02</v>
       </c>
-      <c r="V45" s="20">
+      <c r="V45" s="19">
         <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:22">
       <c r="A49" s="4" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:22">
@@ -3230,18 +3229,18 @@
         <v>2015</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U50" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V50" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:22">
       <c r="B51" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -3260,7 +3259,7 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
       <c r="S51" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T51" s="10"/>
       <c r="U51" s="10"/>
@@ -3268,7 +3267,7 @@
     </row>
     <row r="55" spans="1:22">
       <c r="A55" s="4" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:22">
@@ -3321,18 +3320,18 @@
         <v>2015</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U56" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:22">
       <c r="B57" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -3351,7 +3350,7 @@
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="S57" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T57" s="10"/>
       <c r="U57" s="10"/>
@@ -3359,7 +3358,7 @@
     </row>
     <row r="61" spans="1:22">
       <c r="A61" s="4" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:22">
@@ -3412,18 +3411,18 @@
         <v>2015</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U62" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V62" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:22">
       <c r="B63" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -3442,7 +3441,7 @@
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
       <c r="S63" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T63" s="10"/>
       <c r="U63" s="10"/>
@@ -3450,7 +3449,7 @@
     </row>
     <row r="67" spans="1:22">
       <c r="A67" s="4" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:22">
@@ -3503,18 +3502,18 @@
         <v>2015</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V68" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:22">
       <c r="B69" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -3533,7 +3532,7 @@
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
       <c r="S69" s="9" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="T69" s="10"/>
       <c r="U69" s="10"/>
@@ -3541,7 +3540,7 @@
     </row>
     <row r="73" spans="1:22">
       <c r="A73" s="4" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:22">
@@ -3594,18 +3593,18 @@
         <v>2015</v>
       </c>
       <c r="T74" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U74" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V74" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:22">
       <c r="B75" s="6" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -3619,28 +3618,28 @@
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
       <c r="N75" s="11"/>
-      <c r="O75" s="16">
+      <c r="O75" s="15">
         <v>0</v>
       </c>
       <c r="P75" s="11"/>
       <c r="Q75" s="11"/>
       <c r="R75" s="11"/>
       <c r="S75" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T75" s="21">
+        <v>39</v>
+      </c>
+      <c r="T75" s="20">
         <v>0.03</v>
       </c>
-      <c r="U75" s="22">
+      <c r="U75" s="21">
         <v>0.02</v>
       </c>
-      <c r="V75" s="22">
+      <c r="V75" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="76" spans="1:22">
       <c r="B76" s="6" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -3654,28 +3653,28 @@
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
       <c r="N76" s="11"/>
-      <c r="O76" s="16">
+      <c r="O76" s="15">
         <v>100</v>
       </c>
       <c r="P76" s="11"/>
       <c r="Q76" s="11"/>
       <c r="R76" s="11"/>
       <c r="S76" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T76" s="21">
+        <v>39</v>
+      </c>
+      <c r="T76" s="20">
         <v>0.03</v>
       </c>
-      <c r="U76" s="22">
+      <c r="U76" s="21">
         <v>0.02</v>
       </c>
-      <c r="V76" s="22">
+      <c r="V76" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="77" spans="1:22">
       <c r="B77" s="6" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -3689,28 +3688,28 @@
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
       <c r="N77" s="11"/>
-      <c r="O77" s="16">
+      <c r="O77" s="15">
         <v>100</v>
       </c>
       <c r="P77" s="11"/>
       <c r="Q77" s="11"/>
       <c r="R77" s="11"/>
       <c r="S77" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T77" s="21">
+        <v>39</v>
+      </c>
+      <c r="T77" s="20">
         <v>0.03</v>
       </c>
-      <c r="U77" s="22">
+      <c r="U77" s="21">
         <v>0.02</v>
       </c>
-      <c r="V77" s="22">
+      <c r="V77" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="78" spans="1:22">
       <c r="B78" s="6" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -3724,28 +3723,28 @@
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
-      <c r="O78" s="16">
+      <c r="O78" s="15">
         <v>200</v>
       </c>
       <c r="P78" s="11"/>
       <c r="Q78" s="11"/>
       <c r="R78" s="11"/>
       <c r="S78" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T78" s="21">
+        <v>39</v>
+      </c>
+      <c r="T78" s="20">
         <v>0.03</v>
       </c>
-      <c r="U78" s="22">
+      <c r="U78" s="21">
         <v>0.02</v>
       </c>
-      <c r="V78" s="22">
+      <c r="V78" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:22">
       <c r="B79" s="6" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -3759,28 +3758,28 @@
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
-      <c r="O79" s="16">
+      <c r="O79" s="15">
         <v>300</v>
       </c>
       <c r="P79" s="11"/>
       <c r="Q79" s="11"/>
       <c r="R79" s="11"/>
       <c r="S79" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T79" s="21">
+        <v>39</v>
+      </c>
+      <c r="T79" s="20">
         <v>0.03</v>
       </c>
-      <c r="U79" s="22">
+      <c r="U79" s="21">
         <v>0.02</v>
       </c>
-      <c r="V79" s="22">
+      <c r="V79" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:22">
       <c r="B80" s="6" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -3794,28 +3793,28 @@
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
       <c r="N80" s="11"/>
-      <c r="O80" s="16">
+      <c r="O80" s="15">
         <v>500</v>
       </c>
       <c r="P80" s="11"/>
       <c r="Q80" s="11"/>
       <c r="R80" s="11"/>
       <c r="S80" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T80" s="21">
+        <v>39</v>
+      </c>
+      <c r="T80" s="20">
         <v>0.03</v>
       </c>
-      <c r="U80" s="22">
+      <c r="U80" s="21">
         <v>0.02</v>
       </c>
-      <c r="V80" s="22">
+      <c r="V80" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="84" spans="1:22">
       <c r="A84" s="4" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:22">
@@ -3868,18 +3867,18 @@
         <v>2015</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="U85" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="V85" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:22">
       <c r="B86" s="6" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -3900,21 +3899,21 @@
       <c r="Q86" s="11"/>
       <c r="R86" s="11"/>
       <c r="S86" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T86" s="21">
+        <v>39</v>
+      </c>
+      <c r="T86" s="20">
         <v>0.03</v>
       </c>
-      <c r="U86" s="22">
+      <c r="U86" s="21">
         <v>0.02</v>
       </c>
-      <c r="V86" s="22">
+      <c r="V86" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="87" spans="1:22">
       <c r="B87" s="6" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -3935,21 +3934,21 @@
       <c r="Q87" s="11"/>
       <c r="R87" s="11"/>
       <c r="S87" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T87" s="21">
+        <v>39</v>
+      </c>
+      <c r="T87" s="20">
         <v>0.03</v>
       </c>
-      <c r="U87" s="22">
+      <c r="U87" s="21">
         <v>0.02</v>
       </c>
-      <c r="V87" s="22">
+      <c r="V87" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="88" spans="1:22">
       <c r="B88" s="6" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -3970,21 +3969,21 @@
       <c r="Q88" s="11"/>
       <c r="R88" s="11"/>
       <c r="S88" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T88" s="21">
+        <v>39</v>
+      </c>
+      <c r="T88" s="20">
         <v>0.03</v>
       </c>
-      <c r="U88" s="22">
+      <c r="U88" s="21">
         <v>0.02</v>
       </c>
-      <c r="V88" s="22">
+      <c r="V88" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="89" spans="1:22">
       <c r="B89" s="6" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -4005,21 +4004,21 @@
       <c r="Q89" s="11"/>
       <c r="R89" s="11"/>
       <c r="S89" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T89" s="21">
+        <v>39</v>
+      </c>
+      <c r="T89" s="20">
         <v>0.03</v>
       </c>
-      <c r="U89" s="22">
+      <c r="U89" s="21">
         <v>0.02</v>
       </c>
-      <c r="V89" s="22">
+      <c r="V89" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="90" spans="1:22">
       <c r="B90" s="6" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -4040,21 +4039,21 @@
       <c r="Q90" s="11"/>
       <c r="R90" s="11"/>
       <c r="S90" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T90" s="21">
+        <v>39</v>
+      </c>
+      <c r="T90" s="20">
         <v>0.03</v>
       </c>
-      <c r="U90" s="22">
+      <c r="U90" s="21">
         <v>0.02</v>
       </c>
-      <c r="V90" s="22">
+      <c r="V90" s="21">
         <v>0.05</v>
       </c>
     </row>
     <row r="91" spans="1:22">
       <c r="B91" s="6" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
@@ -4075,22 +4074,21 @@
       <c r="Q91" s="11"/>
       <c r="R91" s="11"/>
       <c r="S91" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T91" s="21">
+        <v>39</v>
+      </c>
+      <c r="T91" s="20">
         <v>0.03</v>
       </c>
-      <c r="U91" s="22">
+      <c r="U91" s="21">
         <v>0.02</v>
       </c>
-      <c r="V91" s="22">
+      <c r="V91" s="21">
         <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4119,36 +4117,36 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>132</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="5" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>135</v>
+        <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4156,25 +4154,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>143</v>
+        <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="J3" s="7" t="b">
         <v>0</v>
@@ -4185,15 +4183,15 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="C8" s="5" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4201,10 +4199,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -4212,10 +4210,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4234,15 +4232,15 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="4" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -4295,7 +4293,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -4304,7 +4302,7 @@
         <v>NSP</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -4333,7 +4331,7 @@
       </c>
       <c r="S3" s="8"/>
       <c r="T3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U3" s="8"/>
     </row>
@@ -4343,7 +4341,7 @@
         <v>NSP</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4372,7 +4370,7 @@
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U4" s="10"/>
     </row>
@@ -4382,7 +4380,7 @@
         <v>ART</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -4390,36 +4388,36 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="14">
-        <v>400</v>
-      </c>
-      <c r="K6" s="14">
-        <v>420</v>
-      </c>
-      <c r="L6" s="14">
-        <v>500</v>
-      </c>
-      <c r="M6" s="14">
-        <v>550</v>
-      </c>
-      <c r="N6" s="14">
-        <v>550</v>
-      </c>
-      <c r="O6" s="14">
-        <v>600</v>
-      </c>
-      <c r="P6" s="14">
-        <v>650</v>
-      </c>
-      <c r="Q6" s="14">
-        <v>670</v>
-      </c>
-      <c r="R6" s="14">
-        <v>800</v>
+      <c r="J6" s="13">
+        <v>30</v>
+      </c>
+      <c r="K6" s="13">
+        <v>50</v>
+      </c>
+      <c r="L6" s="13">
+        <v>130</v>
+      </c>
+      <c r="M6" s="13">
+        <v>150</v>
+      </c>
+      <c r="N6" s="13">
+        <v>350</v>
+      </c>
+      <c r="O6" s="13">
+        <v>450</v>
+      </c>
+      <c r="P6" s="13">
+        <v>620</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>850</v>
+      </c>
+      <c r="R6" s="13">
+        <v>1000</v>
       </c>
       <c r="S6" s="8"/>
       <c r="T6" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U6" s="8"/>
     </row>
@@ -4429,7 +4427,7 @@
         <v>ART</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4466,7 +4464,7 @@
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U7" s="10"/>
     </row>
@@ -4495,7 +4493,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -4548,7 +4546,7 @@
         <v>2015</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -4557,7 +4555,7 @@
         <v>PWID</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D3" s="10">
         <f>D4*0.9</f>
@@ -4621,7 +4619,7 @@
       </c>
       <c r="S3" s="10"/>
       <c r="T3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U3" s="10"/>
     </row>
@@ -4631,7 +4629,7 @@
         <v>PWID</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D4" s="10">
         <v>20000</v>
@@ -4680,7 +4678,7 @@
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U4" s="10"/>
     </row>
@@ -4690,7 +4688,7 @@
         <v>PWID</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D5" s="10">
         <f>D4*1.1</f>
@@ -4754,13 +4752,13 @@
       </c>
       <c r="S5" s="10"/>
       <c r="T5" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U5" s="10"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -4813,7 +4811,7 @@
         <v>2015</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -4822,7 +4820,7 @@
         <v>PWID</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -4841,7 +4839,7 @@
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
       <c r="T12" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U12" s="8"/>
     </row>
@@ -4851,7 +4849,7 @@
         <v>PWID</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D13" s="8">
         <v>0.05</v>
@@ -4886,7 +4884,7 @@
       </c>
       <c r="S13" s="8"/>
       <c r="T13" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U13" s="8"/>
     </row>
@@ -4896,7 +4894,7 @@
         <v>PWID</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -4915,17 +4913,16 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="U14" s="8"/>
     </row>
     <row r="18" spans="10:10">
-      <c r="J18" s="15"/>
+      <c r="J18" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4947,7 +4944,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5000,12 +4997,12 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -5024,7 +5021,7 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T3" s="11">
         <v>3000</v>
@@ -5032,7 +5029,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -5085,12 +5082,12 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="B9" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -5111,13 +5108,13 @@
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T9" s="11"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5170,12 +5167,12 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="B15" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -5194,7 +5191,7 @@
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T15" s="11">
         <v>1200</v>
@@ -5202,7 +5199,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="4" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -5255,12 +5252,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="B21" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -5279,13 +5276,13 @@
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
       <c r="S21" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T21" s="11"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="4" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -5338,12 +5335,12 @@
         <v>2015</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="B27" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -5362,13 +5359,13 @@
       <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
       <c r="S27" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T27" s="11"/>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -5421,12 +5418,12 @@
         <v>2015</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="2:20">
       <c r="B33" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -5445,7 +5442,7 @@
       <c r="Q33" s="11"/>
       <c r="R33" s="11"/>
       <c r="S33" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T33" s="11"/>
     </row>
@@ -5473,7 +5470,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5526,7 +5523,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -5551,7 +5548,7 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T3" s="8">
         <v>0.04</v>
@@ -5559,7 +5556,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -5612,7 +5609,7 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5643,13 +5640,13 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T9" s="8"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5702,7 +5699,7 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -5733,13 +5730,13 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T15" s="8"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="4" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -5792,7 +5789,7 @@
         <v>2015</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -5817,14 +5814,13 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T21" s="8">
         <v>0.08</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5840,15 +5836,15 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5901,7 +5897,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -5936,13 +5932,13 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T3" s="12"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -5995,12 +5991,12 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -6019,7 +6015,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T9" s="12">
         <v>0.5</v>
@@ -6027,7 +6023,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -6080,12 +6076,12 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="B15" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -6122,13 +6118,13 @@
       </c>
       <c r="R15" s="7"/>
       <c r="S15" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T15" s="7"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="4" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -6181,12 +6177,12 @@
         <v>2015</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="B21" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -6215,13 +6211,13 @@
       </c>
       <c r="R21" s="7"/>
       <c r="S21" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T21" s="7"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -6274,12 +6270,12 @@
         <v>2015</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="B27" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -6308,13 +6304,13 @@
       </c>
       <c r="R27" s="7"/>
       <c r="S27" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T27" s="7"/>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -6367,7 +6363,7 @@
         <v>2015</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -6392,7 +6388,7 @@
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T33" s="12">
         <v>0</v>
@@ -6400,7 +6396,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="4" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -6453,12 +6449,12 @@
         <v>2015</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:20">
       <c r="B39" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -6477,13 +6473,13 @@
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="S39" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T39" s="7"/>
     </row>
     <row r="43" spans="1:20">
       <c r="A43" s="4" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -6536,12 +6532,12 @@
         <v>2015</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="4" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:20">
@@ -6594,12 +6590,12 @@
         <v>2015</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="2:20">
       <c r="B50" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -6618,14 +6614,14 @@
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
       <c r="S50" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T50" s="12"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6647,7 +6643,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6700,7 +6696,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6725,7 +6721,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T3" s="7">
         <v>80</v>
@@ -6733,7 +6729,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -6786,7 +6782,7 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -6811,7 +6807,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T9" s="7">
         <v>15</v>
@@ -6819,7 +6815,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -6872,7 +6868,7 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -6897,7 +6893,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T15" s="7">
         <v>0</v>
@@ -6905,7 +6901,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="4" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -6958,7 +6954,7 @@
         <v>2015</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -6989,13 +6985,13 @@
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
       <c r="S21" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T21" s="12"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="4" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -7048,7 +7044,7 @@
         <v>2015</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -7079,13 +7075,13 @@
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T27" s="12"/>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="4" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -7138,7 +7134,7 @@
         <v>2015</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -7163,13 +7159,13 @@
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T33" s="12"/>
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="4" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -7222,11 +7218,10 @@
         <v>2015</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7242,7 +7237,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -7250,7 +7245,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="4" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -7303,7 +7298,7 @@
         <v>2015</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -7336,13 +7331,13 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T3" s="7"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -7395,7 +7390,7 @@
         <v>2015</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -7428,13 +7423,13 @@
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T9" s="12"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -7487,12 +7482,12 @@
         <v>2015</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="B15" s="6" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -7511,14 +7506,13 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="9" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="T15" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>